<commit_message>
fix position of aggr stats
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\muni\studium\04\iv109\iv109\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F663E67C-E624-40C4-8D1A-A0C037D71431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4864207E-2C5A-4ADC-9888-A8DD1EB86E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6FC416FD-78CD-481D-AB5B-9DC8586E8DD5}"/>
   </bookViews>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8955D2D3-9A31-4722-A129-5FF99C596411}">
   <dimension ref="A1:DE241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" zoomScale="61" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="W227" sqref="W227"/>
+    <sheetView tabSelected="1" topLeftCell="BV1" zoomScale="55" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CR18" sqref="CR18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -899,47 +899,47 @@
       </c>
       <c r="BU3" s="1">
         <f t="shared" si="3"/>
-        <v>0.69072791370043296</v>
+        <v>0.6489499999999998</v>
       </c>
       <c r="BV3" s="1">
         <f t="shared" si="3"/>
-        <v>0.53479424046334056</v>
+        <v>0.43968575536223353</v>
       </c>
       <c r="BW3" s="1">
         <f t="shared" si="3"/>
-        <v>0.46042956419339542</v>
+        <v>0.26336665152201733</v>
       </c>
       <c r="BX3" s="1">
         <f t="shared" si="3"/>
-        <v>0.93233541460982183</v>
+        <v>0.64453675534853294</v>
       </c>
       <c r="BY3" s="1">
         <f t="shared" si="3"/>
-        <v>1.0701284596890113</v>
+        <v>0.68491000000000013</v>
       </c>
       <c r="BZ3" s="1">
         <f t="shared" si="3"/>
-        <v>0.92661881034793325</v>
+        <v>0.43827802693917767</v>
       </c>
       <c r="CA3" s="1">
         <f t="shared" si="3"/>
-        <v>0.84837779098519761</v>
+        <v>0.25821534676979546</v>
       </c>
       <c r="CB3" s="1">
-        <f t="shared" si="3"/>
-        <v>1.3424439370157135</v>
+        <f>AVERAGE(CB4:CB220)</f>
+        <v>0.66210288827913277</v>
       </c>
       <c r="CC3" s="1">
         <f t="shared" si="3"/>
-        <v>1.461359985771808</v>
+        <v>0.68310999999999988</v>
       </c>
       <c r="CD3" s="1">
-        <f t="shared" si="3"/>
-        <v>1.3209694522118292</v>
+        <f>AVERAGE(CD4:CD220)</f>
+        <v>0.43974582897754111</v>
       </c>
       <c r="CE3" s="1">
         <f t="shared" si="3"/>
-        <v>1.2443435286799229</v>
+        <v>0.26158081161522007</v>
       </c>
       <c r="CF3" s="1">
         <f t="shared" si="3"/>
@@ -39151,42 +39151,6 @@
       <c r="BN156">
         <v>0.29171764951031598</v>
       </c>
-      <c r="BT156" t="s">
-        <v>13</v>
-      </c>
-      <c r="BU156">
-        <v>5</v>
-      </c>
-      <c r="BV156">
-        <v>10</v>
-      </c>
-      <c r="BW156">
-        <v>20</v>
-      </c>
-      <c r="BX156">
-        <v>30</v>
-      </c>
-      <c r="BY156">
-        <v>40</v>
-      </c>
-      <c r="BZ156">
-        <v>50</v>
-      </c>
-      <c r="CA156">
-        <v>60</v>
-      </c>
-      <c r="CB156">
-        <v>70</v>
-      </c>
-      <c r="CC156">
-        <v>80</v>
-      </c>
-      <c r="CD156">
-        <v>90</v>
-      </c>
-      <c r="CE156">
-        <v>100</v>
-      </c>
     </row>
     <row r="157" spans="15:105" x14ac:dyDescent="0.3">
       <c r="Z157">
@@ -39261,42 +39225,6 @@
       <c r="BN157">
         <v>0.28963660419450299</v>
       </c>
-      <c r="BT157" t="s">
-        <v>14</v>
-      </c>
-      <c r="BU157" s="1">
-        <v>0.55924719744417783</v>
-      </c>
-      <c r="BV157" s="1">
-        <v>0.58043699103738555</v>
-      </c>
-      <c r="BW157" s="1">
-        <v>0.62715039552460405</v>
-      </c>
-      <c r="BX157" s="1">
-        <v>0.64453675534853294</v>
-      </c>
-      <c r="BY157" s="1">
-        <v>0.66210288827913277</v>
-      </c>
-      <c r="BZ157" s="1">
-        <v>0.68731596157143482</v>
-      </c>
-      <c r="CA157" s="1">
-        <v>0.71300000351059778</v>
-      </c>
-      <c r="CB157" s="1">
-        <v>0.7189927476894884</v>
-      </c>
-      <c r="CC157" s="1">
-        <v>0.74771854872442656</v>
-      </c>
-      <c r="CD157" s="1">
-        <v>0.76430122785246712</v>
-      </c>
-      <c r="CE157" s="1">
-        <v>0.7649587638301224</v>
-      </c>
     </row>
     <row r="158" spans="15:105" x14ac:dyDescent="0.3">
       <c r="Z158">
@@ -40904,7 +40832,45 @@
         <v>0.16972293291167001</v>
       </c>
     </row>
-    <row r="236" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="235" spans="4:85" x14ac:dyDescent="0.3">
+      <c r="BV235" t="s">
+        <v>13</v>
+      </c>
+      <c r="BW235">
+        <v>5</v>
+      </c>
+      <c r="BX235">
+        <v>10</v>
+      </c>
+      <c r="BY235">
+        <v>20</v>
+      </c>
+      <c r="BZ235">
+        <v>30</v>
+      </c>
+      <c r="CA235">
+        <v>40</v>
+      </c>
+      <c r="CB235">
+        <v>50</v>
+      </c>
+      <c r="CC235">
+        <v>60</v>
+      </c>
+      <c r="CD235">
+        <v>70</v>
+      </c>
+      <c r="CE235">
+        <v>80</v>
+      </c>
+      <c r="CF235">
+        <v>90</v>
+      </c>
+      <c r="CG235">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="236" spans="4:85" x14ac:dyDescent="0.3">
       <c r="E236" t="s">
         <v>1</v>
       </c>
@@ -40920,8 +40886,44 @@
       <c r="I236" t="s">
         <v>5</v>
       </c>
+      <c r="BV236" t="s">
+        <v>14</v>
+      </c>
+      <c r="BW236" s="1">
+        <v>0.55924719744417783</v>
+      </c>
+      <c r="BX236" s="1">
+        <v>0.58043699103738555</v>
+      </c>
+      <c r="BY236" s="1">
+        <v>0.62715039552460405</v>
+      </c>
+      <c r="BZ236" s="1">
+        <v>0.64453675534853294</v>
+      </c>
+      <c r="CA236" s="1">
+        <v>0.66210288827913277</v>
+      </c>
+      <c r="CB236" s="1">
+        <v>0.68731596157143482</v>
+      </c>
+      <c r="CC236" s="1">
+        <v>0.71300000351059778</v>
+      </c>
+      <c r="CD236" s="1">
+        <v>0.7189927476894884</v>
+      </c>
+      <c r="CE236" s="1">
+        <v>0.74771854872442656</v>
+      </c>
+      <c r="CF236" s="1">
+        <v>0.76430122785246712</v>
+      </c>
+      <c r="CG236" s="1">
+        <v>0.7649587638301224</v>
+      </c>
     </row>
-    <row r="237" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="237" spans="4:85" x14ac:dyDescent="0.3">
       <c r="D237" t="s">
         <v>15</v>
       </c>
@@ -40946,7 +40948,7 @@
         <v>0.50346085015603748</v>
       </c>
     </row>
-    <row r="238" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="238" spans="4:85" x14ac:dyDescent="0.3">
       <c r="D238" t="s">
         <v>16</v>
       </c>
@@ -40966,7 +40968,7 @@
         <v>0.5836228772411276</v>
       </c>
     </row>
-    <row r="239" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="239" spans="4:85" x14ac:dyDescent="0.3">
       <c r="D239" t="s">
         <v>17</v>
       </c>
@@ -40986,7 +40988,7 @@
         <v>0.5904233945434082</v>
       </c>
     </row>
-    <row r="240" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="240" spans="4:85" x14ac:dyDescent="0.3">
       <c r="D240" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
add graph, fix ranges
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\muni\studium\04\iv109\iv109\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4864207E-2C5A-4ADC-9888-A8DD1EB86E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510830C0-5672-4747-8657-79C607975E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6FC416FD-78CD-481D-AB5B-9DC8586E8DD5}"/>
   </bookViews>
@@ -150,6 +150,922 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sk-SK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$BV$236</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean opinion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$BW$235:$CG$235</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$BW$236:$CG$236</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.55924719744417783</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.58043699103738555</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62715039552460405</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64453675534853294</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.66210288827913277</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68731596157143482</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71300000351059778</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7189927476894884</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.74771854872442656</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.76430122785246712</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7649587638301224</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-83F3-4196-948A-C0F2F6AEB2EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="17116592"/>
+        <c:axId val="17117072"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="17116592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sk-SK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="17117072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="17117072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sk-SK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="17116592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sk-SK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>75</xdr:col>
+      <xdr:colOff>233265</xdr:colOff>
+      <xdr:row>237</xdr:row>
+      <xdr:rowOff>31880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>82</xdr:col>
+      <xdr:colOff>559837</xdr:colOff>
+      <xdr:row>251</xdr:row>
+      <xdr:rowOff>162509</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3A08BED-869E-366B-3C9C-C688C21A988B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -471,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8955D2D3-9A31-4722-A129-5FF99C596411}">
   <dimension ref="A1:DE241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BV1" zoomScale="55" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="CR18" sqref="CR18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,6 +1396,7 @@
     <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.77734375" customWidth="1"/>
+    <col min="77" max="77" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:109" x14ac:dyDescent="0.3">
@@ -635,15 +1552,15 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <f>AVERAGE(B4:B100)</f>
-        <v>0.5673702361630949</v>
+        <f>AVERAGE(B4:B200)</f>
+        <v>0.57358153734745421</v>
       </c>
       <c r="C3" s="1">
-        <f>AVERAGE(C4:C100)</f>
-        <v>0.5266205208333784</v>
+        <f t="shared" ref="C3:F3" si="0">AVERAGE(C4:C200)</f>
+        <v>0.54645883469436063</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:X3" si="0">AVERAGE(D4:D100)</f>
+        <f t="shared" si="0"/>
         <v>0.50813637916115073</v>
       </c>
       <c r="E3" s="1">
@@ -657,63 +1574,63 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D3:X3" si="1">AVERAGE(I4:I100)</f>
         <v>0.59687927568733079</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.59450504167088503</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.58594231271456965</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.59418654944916371</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5836228772411276</v>
       </c>
       <c r="O3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.59559783097037933</v>
       </c>
       <c r="P3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.61681443298969041</v>
       </c>
       <c r="Q3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.76447604474303288</v>
       </c>
       <c r="R3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.82583505154639225</v>
       </c>
       <c r="S3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.64876493262596169</v>
       </c>
       <c r="T3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.67200082063907218</v>
       </c>
       <c r="U3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.58974029698389563</v>
       </c>
       <c r="V3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.60190737740969935</v>
       </c>
       <c r="W3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.61855294676939476</v>
       </c>
       <c r="X3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.64196543057906297</v>
       </c>
       <c r="Y3" s="1"/>
@@ -738,63 +1655,63 @@
         <v>0.60027746776435509</v>
       </c>
       <c r="AE3" s="1">
-        <f t="shared" ref="AE3:AS3" si="1">AVERAGE(AE4:AE53)</f>
+        <f t="shared" ref="AE3:AS3" si="2">AVERAGE(AE4:AE53)</f>
         <v>0.62541999999999998</v>
       </c>
       <c r="AF3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.55061291165082016</v>
       </c>
       <c r="AG3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.16800043373515947</v>
       </c>
       <c r="AH3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.59230025939649633</v>
       </c>
       <c r="AI3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.60129353233830796</v>
       </c>
       <c r="AJ3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.561917278685935</v>
       </c>
       <c r="AK3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17554477965426346</v>
       </c>
       <c r="AL3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.60984769376362513</v>
       </c>
       <c r="AM3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.65234131113423477</v>
       </c>
       <c r="AN3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.7607249392993406</v>
       </c>
       <c r="AO3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17369638048082003</v>
       </c>
       <c r="AP3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.59432116455332806</v>
       </c>
       <c r="AQ3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5786069651741288</v>
       </c>
       <c r="AR3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.83272111177932029</v>
       </c>
       <c r="AS3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.18584122637909764</v>
       </c>
       <c r="AU3" s="1">
@@ -818,111 +1735,111 @@
         <v>0.52848230653534356</v>
       </c>
       <c r="AZ3" s="1">
-        <f t="shared" ref="AZ3:BN3" si="2">AVERAGE(AZ4:AZ53)</f>
+        <f t="shared" ref="AZ3:BN3" si="3">AVERAGE(AZ4:AZ53)</f>
         <v>0.51997999999999989</v>
       </c>
       <c r="BA3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.46541006387081801</v>
       </c>
       <c r="BB3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28783412047201939</v>
       </c>
       <c r="BC3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.52518866915434748</v>
       </c>
       <c r="BD3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.52334328358208904</v>
       </c>
       <c r="BE3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.46087630462406504</v>
       </c>
       <c r="BF3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2829665683054261</v>
       </c>
       <c r="BG3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.50365024171869532</v>
       </c>
       <c r="BH3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.51021852237252818</v>
       </c>
       <c r="BI3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.69801248699271534</v>
       </c>
       <c r="BJ3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.29949189262912423</v>
       </c>
       <c r="BK3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.50856422969025483</v>
       </c>
       <c r="BL3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.50581094527363146</v>
       </c>
       <c r="BM3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.79746561768800517</v>
       </c>
       <c r="BN3" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.29398805290130164</v>
       </c>
       <c r="BP3" s="1">
-        <f t="shared" ref="BP3:DE3" si="3">AVERAGE(BP4:BP220)</f>
+        <f t="shared" ref="BP3:DE3" si="4">AVERAGE(BP4:BP220)</f>
         <v>0.58043699103738555</v>
       </c>
       <c r="BQ3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.59774000000000016</v>
       </c>
       <c r="BR3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.44763508687990966</v>
       </c>
       <c r="BS3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.27229651657248249</v>
       </c>
       <c r="BT3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.62715039552460405</v>
       </c>
       <c r="BU3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.6489499999999998</v>
       </c>
       <c r="BV3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.43968575536223353</v>
       </c>
       <c r="BW3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.26336665152201733</v>
       </c>
       <c r="BX3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.64453675534853294</v>
       </c>
       <c r="BY3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.68491000000000013</v>
       </c>
       <c r="BZ3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.43827802693917767</v>
       </c>
       <c r="CA3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.25821534676979546</v>
       </c>
       <c r="CB3" s="1">
@@ -930,7 +1847,7 @@
         <v>0.66210288827913277</v>
       </c>
       <c r="CC3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.68310999999999988</v>
       </c>
       <c r="CD3" s="1">
@@ -938,111 +1855,111 @@
         <v>0.43974582897754111</v>
       </c>
       <c r="CE3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.26158081161522007</v>
       </c>
       <c r="CF3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.68731596157143482</v>
       </c>
       <c r="CG3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.72489000000000003</v>
       </c>
       <c r="CH3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.45721674055980566</v>
       </c>
       <c r="CI3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.24622262685130741</v>
       </c>
       <c r="CJ3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.71300000351059778</v>
       </c>
       <c r="CK3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.74668686868686862</v>
       </c>
       <c r="CL3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.47318173463296725</v>
       </c>
       <c r="CM3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.24868994128275837</v>
       </c>
       <c r="CN3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7189927476894884</v>
       </c>
       <c r="CO3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.75556122448979612</v>
       </c>
       <c r="CP3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.47251736338208383</v>
       </c>
       <c r="CQ3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.24912172009048156</v>
       </c>
       <c r="CR3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.74771854872442656</v>
       </c>
       <c r="CS3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.79907070707070693</v>
       </c>
       <c r="CT3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.48462504229341646</v>
       </c>
       <c r="CU3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.23945525251682215</v>
       </c>
       <c r="CV3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.76430122785246712</v>
       </c>
       <c r="CW3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.81786000000000003</v>
       </c>
       <c r="CX3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.49663391583002764</v>
       </c>
       <c r="CY3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.2355427172988043</v>
       </c>
       <c r="CZ3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7649587638301224</v>
       </c>
       <c r="DA3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.82592253521126813</v>
       </c>
       <c r="DB3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.55924719744417783</v>
       </c>
       <c r="DC3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.57851000000000019</v>
       </c>
       <c r="DD3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.44959128618591693</v>
       </c>
       <c r="DE3" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.26161922377178787</v>
       </c>
     </row>
@@ -40932,8 +41849,8 @@
         <v>0.57863189066525789</v>
       </c>
       <c r="F237" s="1">
-        <f>AVERAGE(C7:C223)</f>
-        <v>0.55273255265245436</v>
+        <f>AVERAGE(C4:C223)</f>
+        <v>0.54645883469436063</v>
       </c>
       <c r="G237" s="1">
         <f>AVERAGE(D7:D223)</f>
@@ -40946,6 +41863,46 @@
       <c r="I237" s="1">
         <f>AVERAGE(F7:F223)</f>
         <v>0.50346085015603748</v>
+      </c>
+      <c r="BX237" s="1">
+        <f>BX236-BW236</f>
+        <v>2.1189793593207717E-2</v>
+      </c>
+      <c r="BY237" s="1">
+        <f t="shared" ref="BY237:CG237" si="5">BY236-BX236</f>
+        <v>4.6713404487218502E-2</v>
+      </c>
+      <c r="BZ237" s="1">
+        <f t="shared" si="5"/>
+        <v>1.7386359823928887E-2</v>
+      </c>
+      <c r="CA237" s="1">
+        <f t="shared" si="5"/>
+        <v>1.7566132930599831E-2</v>
+      </c>
+      <c r="CB237" s="1">
+        <f t="shared" si="5"/>
+        <v>2.5213073292302046E-2</v>
+      </c>
+      <c r="CC237" s="1">
+        <f t="shared" si="5"/>
+        <v>2.568404193916296E-2</v>
+      </c>
+      <c r="CD237" s="1">
+        <f t="shared" si="5"/>
+        <v>5.9927441788906188E-3</v>
+      </c>
+      <c r="CE237" s="1">
+        <f t="shared" si="5"/>
+        <v>2.8725801034938159E-2</v>
+      </c>
+      <c r="CF237" s="1">
+        <f t="shared" si="5"/>
+        <v>1.6582679128040567E-2</v>
+      </c>
+      <c r="CG237" s="1">
+        <f t="shared" si="5"/>
+        <v>6.5753597765527694E-4</v>
       </c>
     </row>
     <row r="238" spans="4:85" x14ac:dyDescent="0.3">
@@ -41037,5 +41994,6 @@
   <ignoredErrors>
     <ignoredError sqref="P3" formulaRange="1"/>
   </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix no ad data
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\muni\studium\04\iv109\iv109\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MUNI\Semester_4\IV109\iv109\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510830C0-5672-4747-8657-79C607975E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA69B6F-BB89-46C1-A8B3-1630447B4399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6FC416FD-78CD-481D-AB5B-9DC8586E8DD5}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{6FC416FD-78CD-481D-AB5B-9DC8586E8DD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -155,7 +155,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="sk-SK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1069,7 +1069,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1388,18 +1388,18 @@
   <dimension ref="A1:DE241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" customWidth="1"/>
-    <col min="77" max="77" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.796875" customWidth="1"/>
+    <col min="77" max="77" width="6.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1547,17 +1547,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:109" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1">
         <f>AVERAGE(B4:B200)</f>
-        <v>0.57358153734745421</v>
+        <v>0.49942132392175881</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:F3" si="0">AVERAGE(C4:C200)</f>
-        <v>0.54645883469436063</v>
+        <v>0.50474091076706196</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" si="0"/>
@@ -1574,7 +1574,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1">
-        <f t="shared" ref="D3:X3" si="1">AVERAGE(I4:I100)</f>
+        <f t="shared" ref="I3:X3" si="1">AVERAGE(I4:I100)</f>
         <v>0.59687927568733079</v>
       </c>
       <c r="J3" s="1">
@@ -1963,12 +1963,12 @@
         <v>0.26161922377178787</v>
       </c>
     </row>
-    <row r="4" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B4">
-        <v>0.38135211211518599</v>
+        <v>0.56890382154866903</v>
       </c>
       <c r="C4">
-        <v>0.301007032660499</v>
+        <v>0.35844069081797397</v>
       </c>
       <c r="D4">
         <v>0.28148849211028798</v>
@@ -2271,12 +2271,12 @@
         <v>0.29353716196507301</v>
       </c>
     </row>
-    <row r="5" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B5">
-        <v>0.42167868494014199</v>
+        <v>0.54357946095922005</v>
       </c>
       <c r="C5">
-        <v>0.34859468209509697</v>
+        <v>0.61615927182317898</v>
       </c>
       <c r="D5">
         <v>0.299406596502092</v>
@@ -2579,12 +2579,12 @@
         <v>0.26292785196372997</v>
       </c>
     </row>
-    <row r="6" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B6">
-        <v>0.42277918984228002</v>
+        <v>0.57044636029701201</v>
       </c>
       <c r="C6">
-        <v>0.356129275560014</v>
+        <v>0.29868222823607998</v>
       </c>
       <c r="D6">
         <v>0.340743213050892</v>
@@ -2887,12 +2887,12 @@
         <v>0.371360922519478</v>
       </c>
     </row>
-    <row r="7" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B7">
-        <v>0.44548853406667499</v>
+        <v>0.40505038588971298</v>
       </c>
       <c r="C7">
-        <v>0.36742849140015399</v>
+        <v>0.45647418320345901</v>
       </c>
       <c r="D7">
         <v>0.34683595691723001</v>
@@ -3195,12 +3195,12 @@
         <v>0.22458918920402399</v>
       </c>
     </row>
-    <row r="8" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B8">
-        <v>0.45171214475139398</v>
+        <v>0.483356967319022</v>
       </c>
       <c r="C8">
-        <v>0.38290217524751802</v>
+        <v>0.44491826702798998</v>
       </c>
       <c r="D8">
         <v>0.35119116175472198</v>
@@ -3503,12 +3503,12 @@
         <v>0.26797240016210699</v>
       </c>
     </row>
-    <row r="9" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B9">
-        <v>0.46999254711371302</v>
+        <v>0.49744015991637502</v>
       </c>
       <c r="C9">
-        <v>0.38894317585328603</v>
+        <v>0.65961831039272401</v>
       </c>
       <c r="D9">
         <v>0.35275564778171498</v>
@@ -3811,12 +3811,12 @@
         <v>0.28248560673461898</v>
       </c>
     </row>
-    <row r="10" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B10">
-        <v>0.47848398729806602</v>
+        <v>0.57226068171080102</v>
       </c>
       <c r="C10">
-        <v>0.39028982042522797</v>
+        <v>0.24159850180560699</v>
       </c>
       <c r="D10">
         <v>0.35681387445901502</v>
@@ -4119,12 +4119,12 @@
         <v>0.29330817533219999</v>
       </c>
     </row>
-    <row r="11" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B11">
-        <v>0.47934264428163498</v>
+        <v>0.41827589750025301</v>
       </c>
       <c r="C11">
-        <v>0.40013475389500203</v>
+        <v>0.592206897801969</v>
       </c>
       <c r="D11">
         <v>0.364134615183757</v>
@@ -4427,12 +4427,12 @@
         <v>0.32022055658895798</v>
       </c>
     </row>
-    <row r="12" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B12">
-        <v>0.485067663010955</v>
+        <v>0.64005641422965798</v>
       </c>
       <c r="C12">
-        <v>0.41118063914109199</v>
+        <v>0.62527620996326905</v>
       </c>
       <c r="D12">
         <v>0.36539365479255997</v>
@@ -4735,12 +4735,12 @@
         <v>0.31369807269785299</v>
       </c>
     </row>
-    <row r="13" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B13">
-        <v>0.48525698692833702</v>
+        <v>0.48748802920905399</v>
       </c>
       <c r="C13">
-        <v>0.411355630515993</v>
+        <v>0.51667776683521305</v>
       </c>
       <c r="D13">
         <v>0.37594251942485402</v>
@@ -5043,12 +5043,12 @@
         <v>0.17865849140012999</v>
       </c>
     </row>
-    <row r="14" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B14">
-        <v>0.48781514370433998</v>
+        <v>0.48079648973922301</v>
       </c>
       <c r="C14">
-        <v>0.41217083106687202</v>
+        <v>0.51240275204827201</v>
       </c>
       <c r="D14">
         <v>0.40160692841124201</v>
@@ -5351,12 +5351,12 @@
         <v>0.23738897227123601</v>
       </c>
     </row>
-    <row r="15" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B15">
-        <v>0.48836859526010201</v>
+        <v>0.49775828068783301</v>
       </c>
       <c r="C15">
-        <v>0.42392195733752402</v>
+        <v>0.43508723076529898</v>
       </c>
       <c r="D15">
         <v>0.40604200807373803</v>
@@ -5659,12 +5659,12 @@
         <v>0.33459887047041598</v>
       </c>
     </row>
-    <row r="16" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:109" x14ac:dyDescent="0.45">
       <c r="B16">
-        <v>0.48861307780615498</v>
+        <v>0.47140999227219099</v>
       </c>
       <c r="C16">
-        <v>0.42528830081243901</v>
+        <v>0.63023877134476802</v>
       </c>
       <c r="D16">
         <v>0.42358378669211699</v>
@@ -5967,12 +5967,12 @@
         <v>0.296941717403785</v>
       </c>
     </row>
-    <row r="17" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B17">
-        <v>0.49772136520851401</v>
+        <v>0.54686898417086605</v>
       </c>
       <c r="C17">
-        <v>0.42605365021403901</v>
+        <v>0.37417129166887703</v>
       </c>
       <c r="D17">
         <v>0.42441960333650602</v>
@@ -6275,12 +6275,12 @@
         <v>0.33395212478131903</v>
       </c>
     </row>
-    <row r="18" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B18">
-        <v>0.49778439385830903</v>
+        <v>0.57081348543055499</v>
       </c>
       <c r="C18">
-        <v>0.42965942087032899</v>
+        <v>0.60309020792270296</v>
       </c>
       <c r="D18">
         <v>0.42477148410687099</v>
@@ -6583,12 +6583,12 @@
         <v>0.25891078148810898</v>
       </c>
     </row>
-    <row r="19" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B19">
-        <v>0.499580986668961</v>
+        <v>0.45518962351032</v>
       </c>
       <c r="C19">
-        <v>0.43424771829735198</v>
+        <v>0.48210180346737003</v>
       </c>
       <c r="D19">
         <v>0.43510974991439499</v>
@@ -6891,12 +6891,12 @@
         <v>0.31429826921447102</v>
       </c>
     </row>
-    <row r="20" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B20">
-        <v>0.50297515385626901</v>
+        <v>0.47361770379246299</v>
       </c>
       <c r="C20">
-        <v>0.43813425698237901</v>
+        <v>0.33068225248271899</v>
       </c>
       <c r="D20">
         <v>0.43562900368187801</v>
@@ -7199,12 +7199,12 @@
         <v>0.35631894916976797</v>
       </c>
     </row>
-    <row r="21" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B21">
-        <v>0.50832723372737798</v>
+        <v>0.47642090947566201</v>
       </c>
       <c r="C21">
-        <v>0.44062605938515897</v>
+        <v>0.68293680493998099</v>
       </c>
       <c r="D21">
         <v>0.43761263681138601</v>
@@ -7507,12 +7507,12 @@
         <v>0.253299787191199</v>
       </c>
     </row>
-    <row r="22" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B22">
-        <v>0.51071882900298604</v>
+        <v>0.50949737219831903</v>
       </c>
       <c r="C22">
-        <v>0.44086834605214897</v>
+        <v>0.29899449854346299</v>
       </c>
       <c r="D22">
         <v>0.438621235293082</v>
@@ -7815,12 +7815,12 @@
         <v>0.282241462755071</v>
       </c>
     </row>
-    <row r="23" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B23">
-        <v>0.51579722108812698</v>
+        <v>0.47569437838326101</v>
       </c>
       <c r="C23">
-        <v>0.44270147523784298</v>
+        <v>0.524128980160943</v>
       </c>
       <c r="D23">
         <v>0.44269932310438198</v>
@@ -8123,12 +8123,12 @@
         <v>0.27259131321080998</v>
       </c>
     </row>
-    <row r="24" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B24">
-        <v>0.51795048099986096</v>
+        <v>0.54181039571478196</v>
       </c>
       <c r="C24">
-        <v>0.44309910847740602</v>
+        <v>0.73065241847599105</v>
       </c>
       <c r="D24">
         <v>0.44635120344698997</v>
@@ -8431,12 +8431,12 @@
         <v>0.233735739128381</v>
       </c>
     </row>
-    <row r="25" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B25">
-        <v>0.52137378361466602</v>
+        <v>0.62348637619382996</v>
       </c>
       <c r="C25">
-        <v>0.45046193455880501</v>
+        <v>0.57144034160368995</v>
       </c>
       <c r="D25">
         <v>0.45059488097942302</v>
@@ -8739,12 +8739,12 @@
         <v>0.263729302589092</v>
       </c>
     </row>
-    <row r="26" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B26">
-        <v>0.52181549100786495</v>
+        <v>0.52361111775371805</v>
       </c>
       <c r="C26">
-        <v>0.45063717165727002</v>
+        <v>0.429488263009977</v>
       </c>
       <c r="D26">
         <v>0.45303931740175402</v>
@@ -9047,12 +9047,12 @@
         <v>0.28862241658159599</v>
       </c>
     </row>
-    <row r="27" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B27">
-        <v>0.52345431470431802</v>
+        <v>0.46943247935343801</v>
       </c>
       <c r="C27">
-        <v>0.457459419538016</v>
+        <v>0.55104859079055402</v>
       </c>
       <c r="D27">
         <v>0.45393399695279002</v>
@@ -9355,12 +9355,12 @@
         <v>0.21922817478147499</v>
       </c>
     </row>
-    <row r="28" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B28">
-        <v>0.52631176705401805</v>
+        <v>0.51529299017738595</v>
       </c>
       <c r="C28">
-        <v>0.45925502603228802</v>
+        <v>0.55611660054573697</v>
       </c>
       <c r="D28">
         <v>0.46166130352543799</v>
@@ -9663,12 +9663,12 @@
         <v>0.23917253401566901</v>
       </c>
     </row>
-    <row r="29" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B29">
-        <v>0.52808494288498198</v>
+        <v>0.41562798263748502</v>
       </c>
       <c r="C29">
-        <v>0.46021733130296999</v>
+        <v>0.62116784080750698</v>
       </c>
       <c r="D29">
         <v>0.46179551757750498</v>
@@ -9971,12 +9971,12 @@
         <v>0.17128584165074301</v>
       </c>
     </row>
-    <row r="30" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B30">
-        <v>0.53059334107485201</v>
+        <v>0.401597595553986</v>
       </c>
       <c r="C30">
-        <v>0.46555682549639399</v>
+        <v>0.53710831078358301</v>
       </c>
       <c r="D30">
         <v>0.46397966290512299</v>
@@ -10279,12 +10279,12 @@
         <v>0.18532607636498299</v>
       </c>
     </row>
-    <row r="31" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B31">
-        <v>0.53070104463549495</v>
+        <v>0.50771470618683701</v>
       </c>
       <c r="C31">
-        <v>0.46621444838954001</v>
+        <v>0.63511355553964999</v>
       </c>
       <c r="D31">
         <v>0.465069179061813</v>
@@ -10587,12 +10587,12 @@
         <v>0.27861724515418002</v>
       </c>
     </row>
-    <row r="32" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B32">
-        <v>0.53575758407906304</v>
+        <v>0.49850134635118298</v>
       </c>
       <c r="C32">
-        <v>0.46978602625302901</v>
+        <v>0.35770259527048498</v>
       </c>
       <c r="D32">
         <v>0.46799477410007401</v>
@@ -10895,12 +10895,12 @@
         <v>0.25277943906925299</v>
       </c>
     </row>
-    <row r="33" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B33">
-        <v>0.53713933696682203</v>
+        <v>0.44349260034434002</v>
       </c>
       <c r="C33">
-        <v>0.47068523469350398</v>
+        <v>0.403068105587434</v>
       </c>
       <c r="D33">
         <v>0.47003466876899203</v>
@@ -11203,12 +11203,12 @@
         <v>0.25928860562900902</v>
       </c>
     </row>
-    <row r="34" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B34">
-        <v>0.54022134720915405</v>
+        <v>0.38204606559898402</v>
       </c>
       <c r="C34">
-        <v>0.47212682993048899</v>
+        <v>0.624685347448661</v>
       </c>
       <c r="D34">
         <v>0.47076697021972902</v>
@@ -11511,12 +11511,12 @@
         <v>0.209215120784147</v>
       </c>
     </row>
-    <row r="35" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B35">
-        <v>0.54022458575839105</v>
+        <v>0.50601933518341802</v>
       </c>
       <c r="C35">
-        <v>0.47593587718520303</v>
+        <v>0.58820737417598301</v>
       </c>
       <c r="D35">
         <v>0.47114563448841601</v>
@@ -11819,12 +11819,12 @@
         <v>0.29716354899257602</v>
       </c>
     </row>
-    <row r="36" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B36">
-        <v>0.542855662027668</v>
+        <v>0.539775699013334</v>
       </c>
       <c r="C36">
-        <v>0.476070623644615</v>
+        <v>0.41334799410421602</v>
       </c>
       <c r="D36">
         <v>0.47466808153393403</v>
@@ -12127,12 +12127,12 @@
         <v>0.248276343890525</v>
       </c>
     </row>
-    <row r="37" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B37">
-        <v>0.54419897464720302</v>
+        <v>0.42422651251531701</v>
       </c>
       <c r="C37">
-        <v>0.48495328542203497</v>
+        <v>0.35080430163074799</v>
       </c>
       <c r="D37">
         <v>0.481783270947581</v>
@@ -12435,12 +12435,12 @@
         <v>0.23769517499064799</v>
       </c>
     </row>
-    <row r="38" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B38">
-        <v>0.54759570813530101</v>
+        <v>0.46261828091692903</v>
       </c>
       <c r="C38">
-        <v>0.48604500794335198</v>
+        <v>0.326973979700868</v>
       </c>
       <c r="D38">
         <v>0.48233254458833402</v>
@@ -12743,12 +12743,12 @@
         <v>0.23856146599327999</v>
       </c>
     </row>
-    <row r="39" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B39">
-        <v>0.55185536792447798</v>
+        <v>0.50608667740658497</v>
       </c>
       <c r="C39">
-        <v>0.486758348365877</v>
+        <v>0.55314892918930403</v>
       </c>
       <c r="D39">
         <v>0.48247827554149703</v>
@@ -13051,12 +13051,12 @@
         <v>0.32227937552751801</v>
       </c>
     </row>
-    <row r="40" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B40">
-        <v>0.55185799996771001</v>
+        <v>0.47009004838071899</v>
       </c>
       <c r="C40">
-        <v>0.48882889475979502</v>
+        <v>0.42101420715097299</v>
       </c>
       <c r="D40">
         <v>0.486306320299356</v>
@@ -13359,12 +13359,12 @@
         <v>0.24496631217985601</v>
       </c>
     </row>
-    <row r="41" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B41">
-        <v>0.55269877347285201</v>
+        <v>0.59289629127633503</v>
       </c>
       <c r="C41">
-        <v>0.49925589558794198</v>
+        <v>0.82976574934230196</v>
       </c>
       <c r="D41">
         <v>0.49095592125863502</v>
@@ -13667,12 +13667,12 @@
         <v>0.29213135982279498</v>
       </c>
     </row>
-    <row r="42" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:109" x14ac:dyDescent="0.45">
       <c r="B42">
-        <v>0.55428063635458402</v>
+        <v>0.50817973414951301</v>
       </c>
       <c r="C42">
-        <v>0.49963376610057902</v>
+        <v>0.50015409350589102</v>
       </c>
       <c r="D42">
         <v>0.49108750270545598</v>
@@ -13975,13 +13975,7 @@
         <v>0.34595684683759997</v>
       </c>
     </row>
-    <row r="43" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B43">
-        <v>0.554366804341339</v>
-      </c>
-      <c r="C43">
-        <v>0.500895531043963</v>
-      </c>
+    <row r="43" spans="2:109" x14ac:dyDescent="0.45">
       <c r="D43">
         <v>0.49283977436509602</v>
       </c>
@@ -14283,13 +14277,7 @@
         <v>0.24913587593004299</v>
       </c>
     </row>
-    <row r="44" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B44">
-        <v>0.55456834005784095</v>
-      </c>
-      <c r="C44">
-        <v>0.50189826260996995</v>
-      </c>
+    <row r="44" spans="2:109" x14ac:dyDescent="0.45">
       <c r="D44">
         <v>0.49302180894568798</v>
       </c>
@@ -14591,13 +14579,7 @@
         <v>0.29216946035103802</v>
       </c>
     </row>
-    <row r="45" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B45">
-        <v>0.55658388214230103</v>
-      </c>
-      <c r="C45">
-        <v>0.50507002185587602</v>
-      </c>
+    <row r="45" spans="2:109" x14ac:dyDescent="0.45">
       <c r="D45">
         <v>0.49913877748693197</v>
       </c>
@@ -14899,13 +14881,7 @@
         <v>0.293215822192188</v>
       </c>
     </row>
-    <row r="46" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B46">
-        <v>0.55679026510768204</v>
-      </c>
-      <c r="C46">
-        <v>0.505684517467203</v>
-      </c>
+    <row r="46" spans="2:109" x14ac:dyDescent="0.45">
       <c r="D46">
         <v>0.49951732819698602</v>
       </c>
@@ -15207,13 +15183,7 @@
         <v>0.28415989042113998</v>
       </c>
     </row>
-    <row r="47" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B47">
-        <v>0.55920495922819302</v>
-      </c>
-      <c r="C47">
-        <v>0.50790607460564297</v>
-      </c>
+    <row r="47" spans="2:109" x14ac:dyDescent="0.45">
       <c r="D47">
         <v>0.50196775808010796</v>
       </c>
@@ -15515,13 +15485,7 @@
         <v>0.28913285544502398</v>
       </c>
     </row>
-    <row r="48" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B48">
-        <v>0.56142352078635105</v>
-      </c>
-      <c r="C48">
-        <v>0.50998694712645598</v>
-      </c>
+    <row r="48" spans="2:109" x14ac:dyDescent="0.45">
       <c r="D48">
         <v>0.50656808992827596</v>
       </c>
@@ -15823,13 +15787,7 @@
         <v>0.17827842146735701</v>
       </c>
     </row>
-    <row r="49" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B49">
-        <v>0.56372274469321004</v>
-      </c>
-      <c r="C49">
-        <v>0.51070840743993595</v>
-      </c>
+    <row r="49" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D49">
         <v>0.506969792297017</v>
       </c>
@@ -16131,13 +16089,7 @@
         <v>0.16638949209943699</v>
       </c>
     </row>
-    <row r="50" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B50">
-        <v>0.56500560279531997</v>
-      </c>
-      <c r="C50">
-        <v>0.51101210013224696</v>
-      </c>
+    <row r="50" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D50">
         <v>0.50713554568840502</v>
       </c>
@@ -16439,13 +16391,7 @@
         <v>0.38351023119586702</v>
       </c>
     </row>
-    <row r="51" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B51">
-        <v>0.56523618325648595</v>
-      </c>
-      <c r="C51">
-        <v>0.51383950406715495</v>
-      </c>
+    <row r="51" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D51">
         <v>0.50801099167660901</v>
       </c>
@@ -16747,13 +16693,7 @@
         <v>0.29718582457090498</v>
       </c>
     </row>
-    <row r="52" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B52">
-        <v>0.56721853931700505</v>
-      </c>
-      <c r="C52">
-        <v>0.51404967395280599</v>
-      </c>
+    <row r="52" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D52">
         <v>0.51013671789100701</v>
       </c>
@@ -17055,13 +16995,7 @@
         <v>0.28341537189403598</v>
       </c>
     </row>
-    <row r="53" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B53">
-        <v>0.56936840258367905</v>
-      </c>
-      <c r="C53">
-        <v>0.51464348666062698</v>
-      </c>
+    <row r="53" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D53">
         <v>0.51343182544599997</v>
       </c>
@@ -17363,13 +17297,7 @@
         <v>0.24057725310543901</v>
       </c>
     </row>
-    <row r="54" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B54">
-        <v>0.570146829534522</v>
-      </c>
-      <c r="C54">
-        <v>0.52065675417853596</v>
-      </c>
+    <row r="54" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D54">
         <v>0.51596117107712103</v>
       </c>
@@ -17671,13 +17599,7 @@
         <v>0.19371456219764299</v>
       </c>
     </row>
-    <row r="55" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B55">
-        <v>0.57100283420659903</v>
-      </c>
-      <c r="C55">
-        <v>0.52708643648642906</v>
-      </c>
+    <row r="55" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D55">
         <v>0.51692957934817996</v>
       </c>
@@ -17979,13 +17901,7 @@
         <v>0.12768009687307</v>
       </c>
     </row>
-    <row r="56" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B56">
-        <v>0.57211804171687397</v>
-      </c>
-      <c r="C56">
-        <v>0.52848805148128997</v>
-      </c>
+    <row r="56" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D56">
         <v>0.52270429916500705</v>
       </c>
@@ -18287,13 +18203,7 @@
         <v>0.23333985624963999</v>
       </c>
     </row>
-    <row r="57" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B57">
-        <v>0.57521455925581599</v>
-      </c>
-      <c r="C57">
-        <v>0.53077731267336303</v>
-      </c>
+    <row r="57" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D57">
         <v>0.52465071761098203</v>
       </c>
@@ -18595,13 +18505,7 @@
         <v>0.280438053218179</v>
       </c>
     </row>
-    <row r="58" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B58">
-        <v>0.57759430388294597</v>
-      </c>
-      <c r="C58">
-        <v>0.53245982212573495</v>
-      </c>
+    <row r="58" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D58">
         <v>0.52585336614450096</v>
       </c>
@@ -18903,13 +18807,7 @@
         <v>0.23373451470555201</v>
       </c>
     </row>
-    <row r="59" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B59">
-        <v>0.583501245085012</v>
-      </c>
-      <c r="C59">
-        <v>0.53335515961747004</v>
-      </c>
+    <row r="59" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D59">
         <v>0.52610970245908495</v>
       </c>
@@ -19211,13 +19109,7 @@
         <v>0.191137589092645</v>
       </c>
     </row>
-    <row r="60" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B60">
-        <v>0.584410566045233</v>
-      </c>
-      <c r="C60">
-        <v>0.53583997080434298</v>
-      </c>
+    <row r="60" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D60">
         <v>0.52662115571961399</v>
       </c>
@@ -19519,13 +19411,7 @@
         <v>0.25401792410458901</v>
       </c>
     </row>
-    <row r="61" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B61">
-        <v>0.58532580192169104</v>
-      </c>
-      <c r="C61">
-        <v>0.54103737154940401</v>
-      </c>
+    <row r="61" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D61">
         <v>0.52702181939660597</v>
       </c>
@@ -19827,13 +19713,7 @@
         <v>0.18129038179434301</v>
       </c>
     </row>
-    <row r="62" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B62">
-        <v>0.58603716333982503</v>
-      </c>
-      <c r="C62">
-        <v>0.548213861567726</v>
-      </c>
+    <row r="62" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D62">
         <v>0.53162900258816603</v>
       </c>
@@ -20135,13 +20015,7 @@
         <v>0.26861648643104902</v>
       </c>
     </row>
-    <row r="63" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B63">
-        <v>0.58666286392690803</v>
-      </c>
-      <c r="C63">
-        <v>0.54949104339997601</v>
-      </c>
+    <row r="63" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D63">
         <v>0.53294147158211402</v>
       </c>
@@ -20443,13 +20317,7 @@
         <v>0.31166374558642801</v>
       </c>
     </row>
-    <row r="64" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B64">
-        <v>0.59002115129272703</v>
-      </c>
-      <c r="C64">
-        <v>0.55183580207051797</v>
-      </c>
+    <row r="64" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D64">
         <v>0.53586174016405397</v>
       </c>
@@ -20751,13 +20619,7 @@
         <v>0.18355084225360699</v>
       </c>
     </row>
-    <row r="65" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B65">
-        <v>0.59318086735684505</v>
-      </c>
-      <c r="C65">
-        <v>0.55259101988637804</v>
-      </c>
+    <row r="65" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D65">
         <v>0.53612919837308404</v>
       </c>
@@ -21059,13 +20921,7 @@
         <v>0.28753625657014298</v>
       </c>
     </row>
-    <row r="66" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B66">
-        <v>0.59532413531477402</v>
-      </c>
-      <c r="C66">
-        <v>0.55370035338996804</v>
-      </c>
+    <row r="66" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D66">
         <v>0.54060306521560098</v>
       </c>
@@ -21367,13 +21223,7 @@
         <v>0.22452372607672999</v>
       </c>
     </row>
-    <row r="67" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B67">
-        <v>0.59533223140387603</v>
-      </c>
-      <c r="C67">
-        <v>0.55510683135498995</v>
-      </c>
+    <row r="67" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D67">
         <v>0.54496835717542003</v>
       </c>
@@ -21675,13 +21525,7 @@
         <v>0.20500315902910099</v>
       </c>
     </row>
-    <row r="68" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B68">
-        <v>0.59683500187620697</v>
-      </c>
-      <c r="C68">
-        <v>0.56171504015254603</v>
-      </c>
+    <row r="68" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D68">
         <v>0.55159197974509999</v>
       </c>
@@ -21983,13 +21827,7 @@
         <v>0.283022746495453</v>
       </c>
     </row>
-    <row r="69" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B69">
-        <v>0.59814337543075002</v>
-      </c>
-      <c r="C69">
-        <v>0.56198374356596603</v>
-      </c>
+    <row r="69" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D69">
         <v>0.55723546095394705</v>
       </c>
@@ -22291,13 +22129,7 @@
         <v>0.36433204318489698</v>
       </c>
     </row>
-    <row r="70" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B70">
-        <v>0.60194023536685703</v>
-      </c>
-      <c r="C70">
-        <v>0.56234656806036099</v>
-      </c>
+    <row r="70" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D70">
         <v>0.55847366943839705</v>
       </c>
@@ -22599,13 +22431,7 @@
         <v>0.20466157718811601</v>
       </c>
     </row>
-    <row r="71" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B71">
-        <v>0.60404811140163395</v>
-      </c>
-      <c r="C71">
-        <v>0.57005240820595005</v>
-      </c>
+    <row r="71" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D71">
         <v>0.56390568926337803</v>
       </c>
@@ -22907,13 +22733,7 @@
         <v>0.266394497067587</v>
       </c>
     </row>
-    <row r="72" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B72">
-        <v>0.60526199743489095</v>
-      </c>
-      <c r="C72">
-        <v>0.58023567310908897</v>
-      </c>
+    <row r="72" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D72">
         <v>0.56597145909018498</v>
       </c>
@@ -23215,13 +23035,7 @@
         <v>0.29711084450707897</v>
       </c>
     </row>
-    <row r="73" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B73">
-        <v>0.60563624045753295</v>
-      </c>
-      <c r="C73">
-        <v>0.58398749134623795</v>
-      </c>
+    <row r="73" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D73">
         <v>0.570237876878952</v>
       </c>
@@ -23523,13 +23337,7 @@
         <v>0.22111944904851299</v>
       </c>
     </row>
-    <row r="74" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B74">
-        <v>0.60807188094613096</v>
-      </c>
-      <c r="C74">
-        <v>0.58488667093728697</v>
-      </c>
+    <row r="74" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D74">
         <v>0.57310252736251499</v>
       </c>
@@ -23831,13 +23639,7 @@
         <v>0.25388605965736399</v>
       </c>
     </row>
-    <row r="75" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B75">
-        <v>0.61144354440885995</v>
-      </c>
-      <c r="C75">
-        <v>0.58718795744811603</v>
-      </c>
+    <row r="75" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D75">
         <v>0.57325926535637595</v>
       </c>
@@ -24139,13 +23941,7 @@
         <v>0.20823342854711999</v>
       </c>
     </row>
-    <row r="76" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B76">
-        <v>0.613479714058493</v>
-      </c>
-      <c r="C76">
-        <v>0.58761874576353301</v>
-      </c>
+    <row r="76" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D76">
         <v>0.57546705989834401</v>
       </c>
@@ -24447,13 +24243,7 @@
         <v>0.31464986372836901</v>
       </c>
     </row>
-    <row r="77" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B77">
-        <v>0.61674530865823296</v>
-      </c>
-      <c r="C77">
-        <v>0.59102369504019003</v>
-      </c>
+    <row r="77" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D77">
         <v>0.58545933385401105</v>
       </c>
@@ -24755,13 +24545,7 @@
         <v>0.22583701254067001</v>
       </c>
     </row>
-    <row r="78" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B78">
-        <v>0.61720224567941995</v>
-      </c>
-      <c r="C78">
-        <v>0.59396406589165396</v>
-      </c>
+    <row r="78" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D78">
         <v>0.58575758494761099</v>
       </c>
@@ -25063,13 +24847,7 @@
         <v>0.34757428680371999</v>
       </c>
     </row>
-    <row r="79" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B79">
-        <v>0.621778785083272</v>
-      </c>
-      <c r="C79">
-        <v>0.60961333443948496</v>
-      </c>
+    <row r="79" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D79">
         <v>0.59101568677225103</v>
       </c>
@@ -25371,13 +25149,7 @@
         <v>0.354363437579997</v>
       </c>
     </row>
-    <row r="80" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B80">
-        <v>0.62377132137116598</v>
-      </c>
-      <c r="C80">
-        <v>0.612672480204139</v>
-      </c>
+    <row r="80" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D80">
         <v>0.59672222061301605</v>
       </c>
@@ -25679,13 +25451,7 @@
         <v>0.259443656822819</v>
       </c>
     </row>
-    <row r="81" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B81">
-        <v>0.62577988400611595</v>
-      </c>
-      <c r="C81">
-        <v>0.61396877077915901</v>
-      </c>
+    <row r="81" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D81">
         <v>0.604311862472378</v>
       </c>
@@ -25987,13 +25753,7 @@
         <v>0.299719176466552</v>
       </c>
     </row>
-    <row r="82" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B82">
-        <v>0.62813179107037598</v>
-      </c>
-      <c r="C82">
-        <v>0.623108441328454</v>
-      </c>
+    <row r="82" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D82">
         <v>0.60487414285150498</v>
       </c>
@@ -26295,13 +26055,7 @@
         <v>0.20686755105034499</v>
       </c>
     </row>
-    <row r="83" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B83">
-        <v>0.62922900747225097</v>
-      </c>
-      <c r="C83">
-        <v>0.62314137054786201</v>
-      </c>
+    <row r="83" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D83">
         <v>0.60680967329243496</v>
       </c>
@@ -26603,13 +26357,7 @@
         <v>0.29498338737743002</v>
       </c>
     </row>
-    <row r="84" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B84">
-        <v>0.629791886054612</v>
-      </c>
-      <c r="C84">
-        <v>0.62389957729484202</v>
-      </c>
+    <row r="84" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D84">
         <v>0.60956877412794097</v>
       </c>
@@ -26911,13 +26659,7 @@
         <v>0.19023158778871299</v>
       </c>
     </row>
-    <row r="85" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B85">
-        <v>0.63566337120733596</v>
-      </c>
-      <c r="C85">
-        <v>0.63602221218339305</v>
-      </c>
+    <row r="85" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D85">
         <v>0.61215558958771099</v>
       </c>
@@ -27219,13 +26961,7 @@
         <v>0.30191800253003098</v>
       </c>
     </row>
-    <row r="86" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B86">
-        <v>0.63591548505727202</v>
-      </c>
-      <c r="C86">
-        <v>0.63974773070564395</v>
-      </c>
+    <row r="86" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D86">
         <v>0.61345585574041195</v>
       </c>
@@ -27527,13 +27263,7 @@
         <v>0.292027470156207</v>
       </c>
     </row>
-    <row r="87" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B87">
-        <v>0.63933914069846398</v>
-      </c>
-      <c r="C87">
-        <v>0.64079450917099601</v>
-      </c>
+    <row r="87" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D87">
         <v>0.61536803250898298</v>
       </c>
@@ -27835,13 +27565,7 @@
         <v>0.248854512173217</v>
       </c>
     </row>
-    <row r="88" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B88">
-        <v>0.63993323756035903</v>
-      </c>
-      <c r="C88">
-        <v>0.64177242994829997</v>
-      </c>
+    <row r="88" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D88">
         <v>0.61666281896027197</v>
       </c>
@@ -28143,13 +27867,7 @@
         <v>0.19356138274958701</v>
       </c>
     </row>
-    <row r="89" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B89">
-        <v>0.64715868671701704</v>
-      </c>
-      <c r="C89">
-        <v>0.64280072109391495</v>
-      </c>
+    <row r="89" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D89">
         <v>0.61875467689825303</v>
       </c>
@@ -28451,13 +28169,7 @@
         <v>0.221405458899919</v>
       </c>
     </row>
-    <row r="90" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B90">
-        <v>0.64743087587732695</v>
-      </c>
-      <c r="C90">
-        <v>0.64323481012774897</v>
-      </c>
+    <row r="90" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D90">
         <v>0.62170336422294803</v>
       </c>
@@ -28759,13 +28471,7 @@
         <v>0.34277454914378003</v>
       </c>
     </row>
-    <row r="91" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B91">
-        <v>0.65090532747978902</v>
-      </c>
-      <c r="C91">
-        <v>0.65279570683836396</v>
-      </c>
+    <row r="91" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D91">
         <v>0.62862068978490104</v>
       </c>
@@ -29067,13 +28773,7 @@
         <v>0.19616785905733999</v>
       </c>
     </row>
-    <row r="92" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B92">
-        <v>0.651987997973001</v>
-      </c>
-      <c r="C92">
-        <v>0.65543021110731003</v>
-      </c>
+    <row r="92" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D92">
         <v>0.66944346876878402</v>
       </c>
@@ -29375,13 +29075,7 @@
         <v>0.24852489002915201</v>
       </c>
     </row>
-    <row r="93" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B93">
-        <v>0.65674974124169205</v>
-      </c>
-      <c r="C93">
-        <v>0.67229355938919599</v>
-      </c>
+    <row r="93" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D93">
         <v>0.68284528808923195</v>
       </c>
@@ -29683,13 +29377,7 @@
         <v>0.24879585041133001</v>
       </c>
     </row>
-    <row r="94" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B94">
-        <v>0.65675423809634303</v>
-      </c>
-      <c r="C94">
-        <v>0.67808832999741497</v>
-      </c>
+    <row r="94" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D94">
         <v>0.68288235537419495</v>
       </c>
@@ -29991,13 +29679,7 @@
         <v>0.22338682465370999</v>
       </c>
     </row>
-    <row r="95" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B95">
-        <v>0.65677591397937396</v>
-      </c>
-      <c r="C95">
-        <v>0.69885531755897701</v>
-      </c>
+    <row r="95" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D95">
         <v>0.705503321094472</v>
       </c>
@@ -30299,13 +29981,7 @@
         <v>0.27987434066148897</v>
       </c>
     </row>
-    <row r="96" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B96">
-        <v>0.67808634121717803</v>
-      </c>
-      <c r="C96">
-        <v>0.70703724454490202</v>
-      </c>
+    <row r="96" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D96">
         <v>0.73801996031130801</v>
       </c>
@@ -30607,13 +30283,7 @@
         <v>0.30443843324418002</v>
       </c>
     </row>
-    <row r="97" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B97">
-        <v>0.68304876383897795</v>
-      </c>
-      <c r="C97">
-        <v>0.70988771969309505</v>
-      </c>
+    <row r="97" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O97">
         <v>0.55406661430486304</v>
       </c>
@@ -30891,13 +30561,7 @@
         <v>0.16435344188699999</v>
       </c>
     </row>
-    <row r="98" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B98">
-        <v>0.68328005475657305</v>
-      </c>
-      <c r="C98">
-        <v>0.71652336280374296</v>
-      </c>
+    <row r="98" spans="4:109" x14ac:dyDescent="0.45">
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -31178,13 +30842,7 @@
         <v>0.266230115030612</v>
       </c>
     </row>
-    <row r="99" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B99">
-        <v>0.68842597851857001</v>
-      </c>
-      <c r="C99">
-        <v>0.72924887751359702</v>
-      </c>
+    <row r="99" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O99">
         <v>0.57440223620015296</v>
       </c>
@@ -31462,13 +31120,7 @@
         <v>0.18293833452168001</v>
       </c>
     </row>
-    <row r="100" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B100">
-        <v>0.688977947182283</v>
-      </c>
-      <c r="C100">
-        <v>0.75529867810917295</v>
-      </c>
+    <row r="100" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O100">
         <v>0.52207158862682101</v>
       </c>
@@ -31746,13 +31398,7 @@
         <v>0.32428384638965402</v>
       </c>
     </row>
-    <row r="101" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B101">
-        <v>0.70107731760006198</v>
-      </c>
-      <c r="C101">
-        <v>0.76315212230426699</v>
-      </c>
+    <row r="101" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O101">
         <v>0.58735731756955001</v>
       </c>
@@ -32030,13 +31676,7 @@
         <v>0.26893210338370599</v>
       </c>
     </row>
-    <row r="102" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B102">
-        <v>0.70490080695692203</v>
-      </c>
-      <c r="C102">
-        <v>0.80042995365123704</v>
-      </c>
+    <row r="102" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O102">
         <v>0.60605855467124303</v>
       </c>
@@ -32302,13 +31942,7 @@
         <v>0.28958734678808901</v>
       </c>
     </row>
-    <row r="103" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B103">
-        <v>0.71564288366241502</v>
-      </c>
-      <c r="C103">
-        <v>0.80305949878961003</v>
-      </c>
+    <row r="103" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O103">
         <v>0.61404237605857304</v>
       </c>
@@ -32550,13 +32184,7 @@
         <v>0.26068771625048798</v>
       </c>
     </row>
-    <row r="104" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="B104">
-        <v>0.775201356053279</v>
-      </c>
-      <c r="C104">
-        <v>0.80478450256740697</v>
-      </c>
+    <row r="104" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O104">
         <v>0.59615726864458596</v>
       </c>
@@ -32714,10 +32342,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="105" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="C105">
-        <v>0.82612033693741105</v>
-      </c>
+    <row r="105" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O105">
         <v>0.67170056267747902</v>
       </c>
@@ -32875,10 +32500,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="106" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="C106">
-        <v>0.86586093195951397</v>
-      </c>
+    <row r="106" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O106">
         <v>0.482131930119924</v>
       </c>
@@ -33036,10 +32658,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="107" spans="2:109" x14ac:dyDescent="0.3">
-      <c r="C107">
-        <v>0.88612094116634199</v>
-      </c>
+    <row r="107" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O107">
         <v>0.61331940542941099</v>
       </c>
@@ -33197,7 +32816,7 @@
         <v>0.95199999999999996</v>
       </c>
     </row>
-    <row r="108" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="108" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O108">
         <v>0.57414751285871102</v>
       </c>
@@ -33355,7 +32974,7 @@
         <v>0.92300000000000004</v>
       </c>
     </row>
-    <row r="109" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="109" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O109">
         <v>0.56764156415108802</v>
       </c>
@@ -33513,7 +33132,7 @@
         <v>0.72199999999999998</v>
       </c>
     </row>
-    <row r="110" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="110" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O110">
         <v>0.54515519863942197</v>
       </c>
@@ -33671,7 +33290,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="111" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="111" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O111">
         <v>0.580146084912599</v>
       </c>
@@ -33829,7 +33448,7 @@
         <v>0.80100000000000005</v>
       </c>
     </row>
-    <row r="112" spans="2:109" x14ac:dyDescent="0.3">
+    <row r="112" spans="4:109" x14ac:dyDescent="0.45">
       <c r="O112">
         <v>0.64390890222590502</v>
       </c>
@@ -33987,7 +33606,7 @@
         <v>0.86099999999999999</v>
       </c>
     </row>
-    <row r="113" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="113" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O113">
         <v>0.69046576661586201</v>
       </c>
@@ -34145,7 +33764,7 @@
         <v>0.97899999999999998</v>
       </c>
     </row>
-    <row r="114" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="114" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O114">
         <v>0.55905337577533598</v>
       </c>
@@ -34303,7 +33922,7 @@
         <v>0.97099999999999997</v>
       </c>
     </row>
-    <row r="115" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="115" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O115">
         <v>0.65346208185863197</v>
       </c>
@@ -34461,7 +34080,7 @@
         <v>0.79300000000000004</v>
       </c>
     </row>
-    <row r="116" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="116" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O116">
         <v>0.57350771491637298</v>
       </c>
@@ -34619,7 +34238,7 @@
         <v>0.97799999999999998</v>
       </c>
     </row>
-    <row r="117" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="117" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O117">
         <v>0.67651434801515498</v>
       </c>
@@ -34777,7 +34396,7 @@
         <v>0.46500000000000002</v>
       </c>
     </row>
-    <row r="118" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="118" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O118">
         <v>0.62742706249469304</v>
       </c>
@@ -34935,7 +34554,7 @@
         <v>0.48499999999999999</v>
       </c>
     </row>
-    <row r="119" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="119" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O119">
         <v>0.74419312741523502</v>
       </c>
@@ -35093,7 +34712,7 @@
         <v>0.73899999999999999</v>
       </c>
     </row>
-    <row r="120" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="120" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O120">
         <v>0.59811600313103697</v>
       </c>
@@ -35251,7 +34870,7 @@
         <v>0.89600000000000002</v>
       </c>
     </row>
-    <row r="121" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="121" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O121">
         <v>0.60038678037632198</v>
       </c>
@@ -35409,7 +35028,7 @@
         <v>0.77200000000000002</v>
       </c>
     </row>
-    <row r="122" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="122" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O122">
         <v>0.68698500911106397</v>
       </c>
@@ -35567,7 +35186,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="123" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="123" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O123">
         <v>0.63294676187889798</v>
       </c>
@@ -35713,7 +35332,7 @@
         <v>0.77600000000000002</v>
       </c>
     </row>
-    <row r="124" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="124" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O124">
         <v>0.60160963445532201</v>
       </c>
@@ -35859,7 +35478,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="125" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="125" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O125">
         <v>0.52348191011685097</v>
       </c>
@@ -36005,7 +35624,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="126" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="126" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O126">
         <v>0.64532139968564795</v>
       </c>
@@ -36151,7 +35770,7 @@
         <v>0.874</v>
       </c>
     </row>
-    <row r="127" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="127" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O127">
         <v>0.59142835519696701</v>
       </c>
@@ -36297,7 +35916,7 @@
         <v>0.57199999999999995</v>
       </c>
     </row>
-    <row r="128" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="128" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O128">
         <v>0.61286743254860199</v>
       </c>
@@ -36443,7 +36062,7 @@
         <v>0.86199999999999999</v>
       </c>
     </row>
-    <row r="129" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="129" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O129">
         <v>0.54581108003282597</v>
       </c>
@@ -36589,7 +36208,7 @@
         <v>0.96899999999999997</v>
       </c>
     </row>
-    <row r="130" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="130" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O130">
         <v>0.62432039044607401</v>
       </c>
@@ -36735,7 +36354,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="131" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="131" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O131">
         <v>0.54399672444488301</v>
       </c>
@@ -36881,7 +36500,7 @@
         <v>0.83299999999999996</v>
       </c>
     </row>
-    <row r="132" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="132" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O132">
         <v>0.62735942986382798</v>
       </c>
@@ -37027,7 +36646,7 @@
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="133" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="133" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O133">
         <v>0.63250846156451701</v>
       </c>
@@ -37173,7 +36792,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="134" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="134" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O134">
         <v>0.62383178920226601</v>
       </c>
@@ -37319,7 +36938,7 @@
         <v>0.75900000000000001</v>
       </c>
     </row>
-    <row r="135" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="135" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O135">
         <v>0.66181920835309704</v>
       </c>
@@ -37465,7 +37084,7 @@
         <v>0.94399999999999995</v>
       </c>
     </row>
-    <row r="136" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="136" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O136">
         <v>0.52892004022234596</v>
       </c>
@@ -37611,7 +37230,7 @@
         <v>0.96399999999999997</v>
       </c>
     </row>
-    <row r="137" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="137" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O137">
         <v>0.53891065758452505</v>
       </c>
@@ -37757,7 +37376,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="138" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="138" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O138">
         <v>0.60513505769040299</v>
       </c>
@@ -37903,7 +37522,7 @@
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="139" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="139" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O139">
         <v>0.65040931303363203</v>
       </c>
@@ -38049,7 +37668,7 @@
         <v>0.91300000000000003</v>
       </c>
     </row>
-    <row r="140" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="140" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O140">
         <v>0.58465848266374498</v>
       </c>
@@ -38195,7 +37814,7 @@
         <v>0.92700000000000005</v>
       </c>
     </row>
-    <row r="141" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="141" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O141">
         <v>0.60263453241448495</v>
       </c>
@@ -38341,7 +37960,7 @@
         <v>0.67900000000000005</v>
       </c>
     </row>
-    <row r="142" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="142" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O142">
         <v>0.51989800517920803</v>
       </c>
@@ -38487,7 +38106,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="143" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="143" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O143">
         <v>0.52545062736533399</v>
       </c>
@@ -38633,7 +38252,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="144" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="144" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O144">
         <v>0.51861468217795004</v>
       </c>
@@ -38779,7 +38398,7 @@
         <v>0.84899999999999998</v>
       </c>
     </row>
-    <row r="145" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="145" spans="15:105" x14ac:dyDescent="0.45">
       <c r="O145">
         <v>0.65798459753466598</v>
       </c>
@@ -38919,7 +38538,7 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="146" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="146" spans="15:105" x14ac:dyDescent="0.45">
       <c r="U146">
         <v>0.63047091517960396</v>
       </c>
@@ -39041,7 +38660,7 @@
         <v>0.274879779691586</v>
       </c>
     </row>
-    <row r="147" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="147" spans="15:105" x14ac:dyDescent="0.45">
       <c r="U147">
         <v>0.54928388474959999</v>
       </c>
@@ -39163,7 +38782,7 @@
         <v>0.28594354632875202</v>
       </c>
     </row>
-    <row r="148" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="148" spans="15:105" x14ac:dyDescent="0.45">
       <c r="U148">
         <v>0.554349703775183</v>
       </c>
@@ -39285,7 +38904,7 @@
         <v>0.33156103365106998</v>
       </c>
     </row>
-    <row r="149" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="149" spans="15:105" x14ac:dyDescent="0.45">
       <c r="U149">
         <v>0.47020924639045097</v>
       </c>
@@ -39407,7 +39026,7 @@
         <v>0.28787559032455001</v>
       </c>
     </row>
-    <row r="150" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="150" spans="15:105" x14ac:dyDescent="0.45">
       <c r="U150">
         <v>0.61289666598647197</v>
       </c>
@@ -39517,7 +39136,7 @@
         <v>0.298010728230032</v>
       </c>
     </row>
-    <row r="151" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="151" spans="15:105" x14ac:dyDescent="0.45">
       <c r="U151">
         <v>0.60257573757899097</v>
       </c>
@@ -39627,7 +39246,7 @@
         <v>0.27560348210049102</v>
       </c>
     </row>
-    <row r="152" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="152" spans="15:105" x14ac:dyDescent="0.45">
       <c r="U152">
         <v>0.56573740338176304</v>
       </c>
@@ -39737,7 +39356,7 @@
         <v>0.30351119404938498</v>
       </c>
     </row>
-    <row r="153" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="153" spans="15:105" x14ac:dyDescent="0.45">
       <c r="U153">
         <v>0.60431173202274302</v>
       </c>
@@ -39847,7 +39466,7 @@
         <v>0.293555212162948</v>
       </c>
     </row>
-    <row r="154" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="154" spans="15:105" x14ac:dyDescent="0.45">
       <c r="Z154">
         <v>0.54824133874582603</v>
       </c>
@@ -39921,7 +39540,7 @@
         <v>0.25692928218794298</v>
       </c>
     </row>
-    <row r="155" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="155" spans="15:105" x14ac:dyDescent="0.45">
       <c r="Z155">
         <v>0.65096361588845797</v>
       </c>
@@ -39995,7 +39614,7 @@
         <v>0.34869045982026697</v>
       </c>
     </row>
-    <row r="156" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="156" spans="15:105" x14ac:dyDescent="0.45">
       <c r="Z156">
         <v>0.60887681591486098</v>
       </c>
@@ -40069,7 +39688,7 @@
         <v>0.29171764951031598</v>
       </c>
     </row>
-    <row r="157" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="157" spans="15:105" x14ac:dyDescent="0.45">
       <c r="Z157">
         <v>0.55352723282465899</v>
       </c>
@@ -40143,7 +39762,7 @@
         <v>0.28963660419450299</v>
       </c>
     </row>
-    <row r="158" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="158" spans="15:105" x14ac:dyDescent="0.45">
       <c r="Z158">
         <v>0.59896357949571699</v>
       </c>
@@ -40217,7 +39836,7 @@
         <v>0.31207000603086898</v>
       </c>
     </row>
-    <row r="159" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="159" spans="15:105" x14ac:dyDescent="0.45">
       <c r="Z159">
         <v>0.551633968903112</v>
       </c>
@@ -40291,7 +39910,7 @@
         <v>0.31339073755206998</v>
       </c>
     </row>
-    <row r="160" spans="15:105" x14ac:dyDescent="0.3">
+    <row r="160" spans="15:105" x14ac:dyDescent="0.45">
       <c r="Z160">
         <v>0.63646461744692995</v>
       </c>
@@ -40341,7 +39960,7 @@
         <v>0.27944110913556103</v>
       </c>
     </row>
-    <row r="161" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="161" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z161">
         <v>0.57016334167810701</v>
       </c>
@@ -40391,7 +40010,7 @@
         <v>0.32531871661339001</v>
       </c>
     </row>
-    <row r="162" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="162" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z162">
         <v>0.641195367440626</v>
       </c>
@@ -40441,7 +40060,7 @@
         <v>0.27534119543734398</v>
       </c>
     </row>
-    <row r="163" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="163" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z163">
         <v>0.56723646643053205</v>
       </c>
@@ -40491,7 +40110,7 @@
         <v>0.28375196660160801</v>
       </c>
     </row>
-    <row r="164" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="164" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z164">
         <v>0.69723996306111102</v>
       </c>
@@ -40541,7 +40160,7 @@
         <v>0.29329545666337797</v>
       </c>
     </row>
-    <row r="165" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="165" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z165">
         <v>0.59257032525398701</v>
       </c>
@@ -40591,7 +40210,7 @@
         <v>0.298340680018368</v>
       </c>
     </row>
-    <row r="166" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="166" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z166">
         <v>0.56195480522987595</v>
       </c>
@@ -40641,7 +40260,7 @@
         <v>0.29266308114740502</v>
       </c>
     </row>
-    <row r="167" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="167" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z167">
         <v>0.66620247565478996</v>
       </c>
@@ -40691,7 +40310,7 @@
         <v>0.301591248082418</v>
       </c>
     </row>
-    <row r="168" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="168" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z168">
         <v>0.59940878095151995</v>
       </c>
@@ -40741,7 +40360,7 @@
         <v>0.27338023816323598</v>
       </c>
     </row>
-    <row r="169" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="169" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z169">
         <v>0.494424536930055</v>
       </c>
@@ -40791,7 +40410,7 @@
         <v>0.32105606007044801</v>
       </c>
     </row>
-    <row r="170" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="170" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z170">
         <v>0.52296452475194399</v>
       </c>
@@ -40841,7 +40460,7 @@
         <v>0.34217026310965698</v>
       </c>
     </row>
-    <row r="171" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="171" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z171">
         <v>0.62338393209264797</v>
       </c>
@@ -40891,7 +40510,7 @@
         <v>0.26069265064453001</v>
       </c>
     </row>
-    <row r="172" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="172" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z172">
         <v>0.58621090244835505</v>
       </c>
@@ -40941,7 +40560,7 @@
         <v>0.26643264842666098</v>
       </c>
     </row>
-    <row r="173" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="173" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z173">
         <v>0.57808594854287199</v>
       </c>
@@ -40979,7 +40598,7 @@
         <v>0.34908230838520299</v>
       </c>
     </row>
-    <row r="174" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="174" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z174">
         <v>0.56090243171523702</v>
       </c>
@@ -41005,7 +40624,7 @@
         <v>0.30279864722557298</v>
       </c>
     </row>
-    <row r="175" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="175" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z175">
         <v>0.56045600617792202</v>
       </c>
@@ -41031,7 +40650,7 @@
         <v>0.288403054823959</v>
       </c>
     </row>
-    <row r="176" spans="26:58" x14ac:dyDescent="0.3">
+    <row r="176" spans="26:58" x14ac:dyDescent="0.45">
       <c r="Z176">
         <v>0.52826224569313396</v>
       </c>
@@ -41057,7 +40676,7 @@
         <v>0.35496984190529601</v>
       </c>
     </row>
-    <row r="177" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="177" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z177">
         <v>0.66218682238085902</v>
       </c>
@@ -41083,7 +40702,7 @@
         <v>0.288722409194201</v>
       </c>
     </row>
-    <row r="178" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="178" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z178">
         <v>0.52955130589048405</v>
       </c>
@@ -41109,7 +40728,7 @@
         <v>0.33355393683520601</v>
       </c>
     </row>
-    <row r="179" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="179" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z179">
         <v>0.63050210711280197</v>
       </c>
@@ -41135,7 +40754,7 @@
         <v>0.281978927512123</v>
       </c>
     </row>
-    <row r="180" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="180" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z180">
         <v>0.61196503064778496</v>
       </c>
@@ -41161,7 +40780,7 @@
         <v>0.27767701195932398</v>
       </c>
     </row>
-    <row r="181" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="181" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z181">
         <v>0.65856780352293598</v>
       </c>
@@ -41187,7 +40806,7 @@
         <v>0.32125519734486202</v>
       </c>
     </row>
-    <row r="182" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="182" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z182">
         <v>0.53984449561763204</v>
       </c>
@@ -41213,7 +40832,7 @@
         <v>0.28282606249932501</v>
       </c>
     </row>
-    <row r="183" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="183" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z183">
         <v>0.64625769677416001</v>
       </c>
@@ -41239,7 +40858,7 @@
         <v>0.28451293855764598</v>
       </c>
     </row>
-    <row r="184" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="184" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z184">
         <v>0.67608112290003997</v>
       </c>
@@ -41265,7 +40884,7 @@
         <v>0.23422347626793599</v>
       </c>
     </row>
-    <row r="185" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="185" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z185">
         <v>0.54053793890365898</v>
       </c>
@@ -41291,7 +40910,7 @@
         <v>0.25547445860509699</v>
       </c>
     </row>
-    <row r="186" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="186" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z186">
         <v>0.62998928651753805</v>
       </c>
@@ -41317,7 +40936,7 @@
         <v>0.304535497859107</v>
       </c>
     </row>
-    <row r="187" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="187" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z187">
         <v>0.56077533378974997</v>
       </c>
@@ -41343,7 +40962,7 @@
         <v>0.25623782331040101</v>
       </c>
     </row>
-    <row r="188" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="188" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z188">
         <v>0.61069216086801603</v>
       </c>
@@ -41369,7 +40988,7 @@
         <v>0.259712898965136</v>
       </c>
     </row>
-    <row r="189" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="189" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z189">
         <v>0.60291963989946895</v>
       </c>
@@ -41395,7 +41014,7 @@
         <v>0.335672579089689</v>
       </c>
     </row>
-    <row r="190" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="190" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z190">
         <v>0.56964630901796498</v>
       </c>
@@ -41421,7 +41040,7 @@
         <v>0.28750806733907502</v>
       </c>
     </row>
-    <row r="191" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="191" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z191">
         <v>0.59528017702803104</v>
       </c>
@@ -41447,7 +41066,7 @@
         <v>0.30539180344195199</v>
       </c>
     </row>
-    <row r="192" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="192" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z192">
         <v>0.615414471195038</v>
       </c>
@@ -41473,7 +41092,7 @@
         <v>0.25337195851736699</v>
       </c>
     </row>
-    <row r="193" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="193" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z193">
         <v>0.54464969614299796</v>
       </c>
@@ -41499,7 +41118,7 @@
         <v>0.24197903284432101</v>
       </c>
     </row>
-    <row r="194" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="194" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z194">
         <v>0.61298915877188198</v>
       </c>
@@ -41525,7 +41144,7 @@
         <v>0.28475905769656601</v>
       </c>
     </row>
-    <row r="195" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="195" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z195">
         <v>0.63791843844637797</v>
       </c>
@@ -41539,7 +41158,7 @@
         <v>0.14596331225748199</v>
       </c>
     </row>
-    <row r="196" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="196" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z196">
         <v>0.52217415548865398</v>
       </c>
@@ -41553,7 +41172,7 @@
         <v>0.177545078316314</v>
       </c>
     </row>
-    <row r="197" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="197" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z197">
         <v>0.63422151763964096</v>
       </c>
@@ -41567,7 +41186,7 @@
         <v>0.18763116605888899</v>
       </c>
     </row>
-    <row r="198" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="198" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z198">
         <v>0.52715839014578303</v>
       </c>
@@ -41581,7 +41200,7 @@
         <v>0.16477762012519701</v>
       </c>
     </row>
-    <row r="199" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="199" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z199">
         <v>0.56400244619278495</v>
       </c>
@@ -41595,7 +41214,7 @@
         <v>0.23181094117659601</v>
       </c>
     </row>
-    <row r="200" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="200" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z200">
         <v>0.62495867637098401</v>
       </c>
@@ -41609,7 +41228,7 @@
         <v>0.14404397654418299</v>
       </c>
     </row>
-    <row r="201" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="201" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z201">
         <v>0.62428955632826599</v>
       </c>
@@ -41623,7 +41242,7 @@
         <v>0.168013207116985</v>
       </c>
     </row>
-    <row r="202" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="202" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z202">
         <v>0.64369903325848399</v>
       </c>
@@ -41637,7 +41256,7 @@
         <v>0.18525129104612301</v>
       </c>
     </row>
-    <row r="203" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="203" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z203">
         <v>0.70273990298233202</v>
       </c>
@@ -41651,7 +41270,7 @@
         <v>0.16346537851294499</v>
       </c>
     </row>
-    <row r="204" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="204" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z204">
         <v>0.66079570065749804</v>
       </c>
@@ -41665,7 +41284,7 @@
         <v>0.17714466623096101</v>
       </c>
     </row>
-    <row r="205" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="205" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z205">
         <v>0.66137579622487597</v>
       </c>
@@ -41679,7 +41298,7 @@
         <v>0.18179455214627199</v>
       </c>
     </row>
-    <row r="206" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="206" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z206">
         <v>0.67867311671692698</v>
       </c>
@@ -41693,7 +41312,7 @@
         <v>0.179038322525784</v>
       </c>
     </row>
-    <row r="207" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="207" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z207">
         <v>0.52181294270704004</v>
       </c>
@@ -41707,7 +41326,7 @@
         <v>0.161257577742729</v>
       </c>
     </row>
-    <row r="208" spans="26:50" x14ac:dyDescent="0.3">
+    <row r="208" spans="26:50" x14ac:dyDescent="0.45">
       <c r="Z208">
         <v>0.58547936780038401</v>
       </c>
@@ -41721,7 +41340,7 @@
         <v>0.18178958279263599</v>
       </c>
     </row>
-    <row r="209" spans="26:29" x14ac:dyDescent="0.3">
+    <row r="209" spans="26:29" x14ac:dyDescent="0.45">
       <c r="Z209">
         <v>0.61456007120936496</v>
       </c>
@@ -41735,7 +41354,7 @@
         <v>0.152753380294091</v>
       </c>
     </row>
-    <row r="210" spans="26:29" x14ac:dyDescent="0.3">
+    <row r="210" spans="26:29" x14ac:dyDescent="0.45">
       <c r="Z210">
         <v>0.60726499638134601</v>
       </c>
@@ -41749,7 +41368,7 @@
         <v>0.16972293291167001</v>
       </c>
     </row>
-    <row r="235" spans="4:85" x14ac:dyDescent="0.3">
+    <row r="235" spans="4:85" x14ac:dyDescent="0.45">
       <c r="BV235" t="s">
         <v>13</v>
       </c>
@@ -41787,7 +41406,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="236" spans="4:85" x14ac:dyDescent="0.3">
+    <row r="236" spans="4:85" x14ac:dyDescent="0.45">
       <c r="E236" t="s">
         <v>1</v>
       </c>
@@ -41840,29 +41459,29 @@
         <v>0.7649587638301224</v>
       </c>
     </row>
-    <row r="237" spans="4:85" x14ac:dyDescent="0.3">
+    <row r="237" spans="4:85" x14ac:dyDescent="0.45">
       <c r="D237" t="s">
         <v>15</v>
       </c>
       <c r="E237" s="1">
-        <f>AVERAGE(B7:B223)</f>
-        <v>0.57863189066525789</v>
+        <f>AVERAGE(B4:B223)</f>
+        <v>0.49942132392175881</v>
       </c>
       <c r="F237" s="1">
         <f>AVERAGE(C4:C223)</f>
-        <v>0.54645883469436063</v>
+        <v>0.50474091076706196</v>
       </c>
       <c r="G237" s="1">
-        <f>AVERAGE(D7:D223)</f>
-        <v>0.51483383289248619</v>
+        <f>AVERAGE(D4:D223)</f>
+        <v>0.50813637916115073</v>
       </c>
       <c r="H237" s="1">
-        <f>AVERAGE(E7:E223)</f>
-        <v>0.49835710470044348</v>
+        <f>AVERAGE(E4:E223)</f>
+        <v>0.49456767877070307</v>
       </c>
       <c r="I237" s="1">
-        <f>AVERAGE(F7:F223)</f>
-        <v>0.50346085015603748</v>
+        <f>AVERAGE(F4:F223)</f>
+        <v>0.4989440372507567</v>
       </c>
       <c r="BX237" s="1">
         <f>BX236-BW236</f>
@@ -41905,7 +41524,7 @@
         <v>6.5753597765527694E-4</v>
       </c>
     </row>
-    <row r="238" spans="4:85" x14ac:dyDescent="0.3">
+    <row r="238" spans="4:85" x14ac:dyDescent="0.45">
       <c r="D238" t="s">
         <v>16</v>
       </c>
@@ -41925,7 +41544,7 @@
         <v>0.5836228772411276</v>
       </c>
     </row>
-    <row r="239" spans="4:85" x14ac:dyDescent="0.3">
+    <row r="239" spans="4:85" x14ac:dyDescent="0.45">
       <c r="D239" t="s">
         <v>17</v>
       </c>
@@ -41945,7 +41564,7 @@
         <v>0.5904233945434082</v>
       </c>
     </row>
-    <row r="240" spans="4:85" x14ac:dyDescent="0.3">
+    <row r="240" spans="4:85" x14ac:dyDescent="0.45">
       <c r="D240" t="s">
         <v>18</v>
       </c>
@@ -41965,7 +41584,7 @@
         <v>0.50856422969025483</v>
       </c>
     </row>
-    <row r="241" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="241" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D241" t="s">
         <v>19</v>
       </c>

</xml_diff>